<commit_message>
Auto update FY dropdowns
</commit_message>
<xml_diff>
--- a/templates/discharges-template.xlsx
+++ b/templates/discharges-template.xlsx
@@ -811,21 +811,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -846,6 +831,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2319,11 +2319,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="5" dropStyle="combo" dx="16" fmlaLink="$A$5" fmlaRange="lookup!$F$1:$F$3" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="16" fmlaLink="$A$5" fmlaRange="fy_list" noThreeD="1" sel="0" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="16" fmlaLink="$A$7" fmlaRange="lookup!$F$1:$F$3" noThreeD="1" sel="3" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="3" dropStyle="combo" dx="16" fmlaLink="$A$7" fmlaRange="fy_list" noThreeD="1" sel="0" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3044,35 +3044,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="str">
+      <c r="A1" s="68" t="str">
         <f>"These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland."</f>
         <v>These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland.</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
       <c r="J1" s="10"/>
       <c r="L1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
@@ -3099,165 +3099,165 @@
       <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
       <c r="J5" s="51"/>
     </row>
     <row r="6" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
       <c r="J6" s="51"/>
     </row>
     <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="68"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="63"/>
+      <c r="H9" s="63"/>
+      <c r="I9" s="63"/>
       <c r="J9" s="50" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="63"/>
       <c r="J10" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="72"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3285,31 +3285,31 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -3363,17 +3363,17 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
       <c r="J22" s="9"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3462,6 +3462,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A22:I22"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A12:H12"/>
@@ -3473,11 +3478,6 @@
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A22:I22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A14" location="'Tab 1'!A1" display="Tab 1"/>
@@ -3590,7 +3590,7 @@
     </row>
     <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>45</v>
@@ -4187,7 +4187,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>

</xml_diff>

<commit_message>
Update text for care home report
</commit_message>
<xml_diff>
--- a/templates/discharges-template.xlsx
+++ b/templates/discharges-template.xlsx
@@ -292,9 +292,6 @@
     <t>Link to report</t>
   </si>
   <si>
-    <t>On 28 October 2020, Public Health Scotland published a report on "Discharges from NHSScotland hospitals to care homes" for the period 1 March to 31 May 2020. The report includes figures for delayed discharges to care homes across this time period and can be found here:</t>
-  </si>
-  <si>
     <t>Public Health Scotland's latest annual publication (including summary, full report and data tables) was released on 17 November 2020 and is available here:</t>
   </si>
   <si>
@@ -327,6 +324,9 @@
   </si>
   <si>
     <t>Latest CY</t>
+  </si>
+  <si>
+    <t>On 28 October 2020, Public Health Scotland published a report on "Discharges from NHSScotland hospitals to care homes" for the period 1 March to 31 May 2020. A revision to this publication was published on 21 April 2021. The report includes figures for delayed discharges to care homes across this time period. The latest publication can be found here:</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -791,9 +791,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -811,6 +808,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -831,21 +843,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -954,7 +951,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1412,7 +1408,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3044,35 +3039,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="str">
+      <c r="A1" s="72" t="str">
         <f>"These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland."</f>
         <v>These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland.</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
       <c r="J1" s="10"/>
       <c r="L1" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
@@ -3099,165 +3094,165 @@
       <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="51"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="51"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="63"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
       <c r="J8" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
       <c r="J9" s="50" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
       <c r="J10" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="64"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="66"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="70"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="62"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="62"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3285,31 +3280,31 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="63"/>
+      <c r="I18" s="63"/>
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
+      <c r="A19" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -3363,17 +3358,17 @@
       <c r="V21" s="9"/>
     </row>
     <row r="22" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
       <c r="J22" s="9"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
@@ -3462,11 +3457,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A22:I22"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A12:H12"/>
@@ -3478,6 +3468,11 @@
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A9:I9"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A22:I22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A14" location="'Tab 1'!A1" display="Tab 1"/>
@@ -3534,30 +3529,30 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="76" t="e">
+      <c r="B3" s="75" t="e">
         <f>"All delay reasons, "&amp; $A$6</f>
         <v>#NAME?</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
@@ -3571,7 +3566,7 @@
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:15" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -3630,18 +3625,18 @@
         <f>LEFT($A$6, 4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="77" t="s">
+      <c r="D7" s="77"/>
+      <c r="E7" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="78"/>
+      <c r="F7" s="77"/>
       <c r="G7" s="28"/>
     </row>
     <row r="8" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="e">
+      <c r="A8" s="53" t="e">
         <f>"20"&amp;RIGHT($A$6, 2)</f>
         <v>#NAME?</v>
       </c>
@@ -3665,7 +3660,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="55" t="e">
+      <c r="A9" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B9, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3673,7 +3668,7 @@
         <f xml:space="preserve"> "April " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9" s="52" t="str">
+      <c r="C9" s="51" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3681,7 +3676,7 @@
         <f t="shared" ref="D9:D20" si="0">IFERROR($C9/$G9, "-")</f>
         <v>-</v>
       </c>
-      <c r="E9" s="52" t="str">
+      <c r="E9" s="51" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3689,13 +3684,13 @@
         <f t="shared" ref="F9:F20" si="1">IFERROR($E9/$G9, "-")</f>
         <v>-</v>
       </c>
-      <c r="G9" s="52" t="str">
+      <c r="G9" s="51" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="e">
+      <c r="A10" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B10, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3703,7 +3698,7 @@
         <f xml:space="preserve"> "May " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C10" s="52" t="str">
+      <c r="C10" s="51" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3711,7 +3706,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E10" s="52" t="str">
+      <c r="E10" s="51" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3719,13 +3714,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G10" s="52" t="str">
+      <c r="G10" s="51" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="55" t="e">
+      <c r="A11" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B11, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3733,7 +3728,7 @@
         <f xml:space="preserve"> "June " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C11" s="52" t="str">
+      <c r="C11" s="51" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3741,7 +3736,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E11" s="52" t="str">
+      <c r="E11" s="51" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3749,13 +3744,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G11" s="52" t="str">
+      <c r="G11" s="51" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="e">
+      <c r="A12" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B12, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3763,7 +3758,7 @@
         <f xml:space="preserve"> "July " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C12" s="52" t="str">
+      <c r="C12" s="51" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3771,7 +3766,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E12" s="52" t="str">
+      <c r="E12" s="51" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3779,13 +3774,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G12" s="52" t="str">
+      <c r="G12" s="51" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="55" t="e">
+      <c r="A13" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B13, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3793,7 +3788,7 @@
         <f xml:space="preserve"> "August " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C13" s="52" t="str">
+      <c r="C13" s="51" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3801,7 +3796,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E13" s="52" t="str">
+      <c r="E13" s="51" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3809,13 +3804,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G13" s="52" t="str">
+      <c r="G13" s="51" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="55" t="e">
+      <c r="A14" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B14, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3823,7 +3818,7 @@
         <f xml:space="preserve"> "September " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C14" s="52" t="str">
+      <c r="C14" s="51" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3831,7 +3826,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E14" s="52" t="str">
+      <c r="E14" s="51" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3839,13 +3834,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G14" s="52" t="str">
+      <c r="G14" s="51" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="e">
+      <c r="A15" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B15, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3853,7 +3848,7 @@
         <f xml:space="preserve"> "October " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C15" s="52" t="str">
+      <c r="C15" s="51" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3861,7 +3856,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E15" s="52" t="str">
+      <c r="E15" s="51" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3869,13 +3864,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G15" s="52" t="str">
+      <c r="G15" s="51" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="e">
+      <c r="A16" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B16, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3883,7 +3878,7 @@
         <f xml:space="preserve"> "November " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C16" s="52" t="str">
+      <c r="C16" s="51" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3891,7 +3886,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E16" s="52" t="str">
+      <c r="E16" s="51" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3899,13 +3894,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G16" s="52" t="str">
+      <c r="G16" s="51" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="e">
+      <c r="A17" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B17, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3913,7 +3908,7 @@
         <f xml:space="preserve"> "December " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C17" s="52" t="str">
+      <c r="C17" s="51" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3921,7 +3916,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E17" s="52" t="str">
+      <c r="E17" s="51" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3929,13 +3924,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G17" s="52" t="str">
+      <c r="G17" s="51" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="e">
+      <c r="A18" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B18, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3943,7 +3938,7 @@
         <f xml:space="preserve"> "January " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C18" s="52" t="str">
+      <c r="C18" s="51" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3951,7 +3946,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E18" s="52" t="str">
+      <c r="E18" s="51" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3959,13 +3954,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G18" s="52" t="str">
+      <c r="G18" s="51" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="e">
+      <c r="A19" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B19, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -3973,7 +3968,7 @@
         <f xml:space="preserve"> "February " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C19" s="52" t="str">
+      <c r="C19" s="51" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3981,7 +3976,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E19" s="52" t="str">
+      <c r="E19" s="51" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -3989,13 +3984,13 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G19" s="52" t="str">
+      <c r="G19" s="51" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="e">
+      <c r="A20" s="55" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B20, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4003,7 +3998,7 @@
         <f xml:space="preserve"> "March " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C20" s="52" t="str">
+      <c r="C20" s="51" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -4011,7 +4006,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E20" s="52" t="str">
+      <c r="E20" s="51" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -4019,7 +4014,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G20" s="52" t="str">
+      <c r="G20" s="51" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
@@ -4057,14 +4052,14 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="75" t="s">
+      <c r="B27" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
     </row>
     <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4151,23 +4146,23 @@
       <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="e">
+      <c r="B2" s="75" t="e">
         <f>"Tab 2 - Discharges from hospital following period of delay to Home or to Placement; by Health Board; " &amp; A12</f>
         <v>#NAME?</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
@@ -4202,14 +4197,14 @@
         <v>#NAME?</v>
       </c>
       <c r="B8" s="28"/>
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="78"/>
-      <c r="E8" s="77" t="s">
+      <c r="D8" s="77"/>
+      <c r="E8" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="78"/>
+      <c r="F8" s="77"/>
       <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:15" ht="27" x14ac:dyDescent="0.25">
@@ -4269,7 +4264,7 @@
       <c r="B11" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="52" t="e">
+      <c r="C11" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4277,7 +4272,7 @@
         <f>IFERROR(C11/G11, "-")</f>
         <v>-</v>
       </c>
-      <c r="E11" s="52" t="e">
+      <c r="E11" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4285,7 +4280,7 @@
         <f>IFERROR(E11/G11, "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="52" t="e">
+      <c r="G11" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4298,7 +4293,7 @@
       <c r="B12" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="52" t="e">
+      <c r="C12" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4306,7 +4301,7 @@
         <f t="shared" ref="D12:D24" si="0">IFERROR(C12/G12, "-")</f>
         <v>-</v>
       </c>
-      <c r="E12" s="52" t="e">
+      <c r="E12" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4314,7 +4309,7 @@
         <f t="shared" ref="F12:F24" si="1">IFERROR(E12/G12, "-")</f>
         <v>-</v>
       </c>
-      <c r="G12" s="52" t="e">
+      <c r="G12" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4323,7 +4318,7 @@
       <c r="B13" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="52" t="e">
+      <c r="C13" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4331,7 +4326,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E13" s="52" t="e">
+      <c r="E13" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4339,7 +4334,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G13" s="52" t="e">
+      <c r="G13" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4348,7 +4343,7 @@
       <c r="B14" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="52" t="e">
+      <c r="C14" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4356,7 +4351,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E14" s="52" t="e">
+      <c r="E14" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4364,7 +4359,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G14" s="52" t="e">
+      <c r="G14" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4373,7 +4368,7 @@
       <c r="B15" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="52" t="e">
+      <c r="C15" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4381,7 +4376,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E15" s="52" t="e">
+      <c r="E15" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4389,7 +4384,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G15" s="52" t="e">
+      <c r="G15" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4398,7 +4393,7 @@
       <c r="B16" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="52" t="e">
+      <c r="C16" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4406,7 +4401,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E16" s="52" t="e">
+      <c r="E16" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4414,7 +4409,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G16" s="52" t="e">
+      <c r="G16" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4423,7 +4418,7 @@
       <c r="B17" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="52" t="e">
+      <c r="C17" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4431,7 +4426,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E17" s="52" t="e">
+      <c r="E17" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4439,7 +4434,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G17" s="52" t="e">
+      <c r="G17" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4448,7 +4443,7 @@
       <c r="B18" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="52" t="e">
+      <c r="C18" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4456,7 +4451,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E18" s="52" t="e">
+      <c r="E18" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4464,7 +4459,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G18" s="52" t="e">
+      <c r="G18" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4473,7 +4468,7 @@
       <c r="B19" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="52" t="e">
+      <c r="C19" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4481,7 +4476,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E19" s="52" t="e">
+      <c r="E19" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4489,7 +4484,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G19" s="52" t="e">
+      <c r="G19" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4498,7 +4493,7 @@
       <c r="B20" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="52" t="e">
+      <c r="C20" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4506,7 +4501,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E20" s="52" t="e">
+      <c r="E20" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4514,7 +4509,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G20" s="52" t="e">
+      <c r="G20" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4523,7 +4518,7 @@
       <c r="B21" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="52" t="e">
+      <c r="C21" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4531,7 +4526,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E21" s="52" t="e">
+      <c r="E21" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4539,7 +4534,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G21" s="52" t="e">
+      <c r="G21" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4548,7 +4543,7 @@
       <c r="B22" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="52" t="e">
+      <c r="C22" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4556,7 +4551,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E22" s="52" t="e">
+      <c r="E22" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4564,7 +4559,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G22" s="52" t="e">
+      <c r="G22" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4573,7 +4568,7 @@
       <c r="B23" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="52" t="e">
+      <c r="C23" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4581,7 +4576,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E23" s="52" t="e">
+      <c r="E23" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4589,7 +4584,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G23" s="52" t="e">
+      <c r="G23" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4598,7 +4593,7 @@
       <c r="B24" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="52" t="e">
+      <c r="C24" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4606,7 +4601,7 @@
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E24" s="52" t="e">
+      <c r="E24" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4614,7 +4609,7 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G24" s="52" t="e">
+      <c r="G24" s="51" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
@@ -4654,15 +4649,15 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="79" t="str">
+      <c r="B31" s="78" t="str">
         <f>'Tab 1'!B27</f>
         <v>3. These figures are a subset of the total number of discharges from hospital and include only those people who experienced a period of delay prior to their discharge and were discharged home or to a placement (delays in hospital that ended due to death are not included).</v>
       </c>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4736,286 +4731,286 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="60" customWidth="1"/>
-    <col min="3" max="3" width="3" style="60" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="60" customWidth="1"/>
-    <col min="5" max="5" width="2" style="60" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="60" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="60" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="60" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="60"/>
-    <col min="12" max="12" width="3" style="60" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="60" customWidth="1"/>
-    <col min="14" max="14" width="3" style="60" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="60" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="60" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="60"/>
-    <col min="18" max="18" width="15.42578125" style="60" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="60"/>
+    <col min="1" max="1" width="3" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="3" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="59" customWidth="1"/>
+    <col min="5" max="5" width="2" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="59" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="59" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="59"/>
+    <col min="12" max="12" width="3" style="59" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="59" customWidth="1"/>
+    <col min="14" max="14" width="3" style="59" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="59" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="59"/>
+    <col min="18" max="18" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="59"/>
-      <c r="H1" s="60" t="s">
+      <c r="B1" s="58"/>
+      <c r="H1" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="60" t="e">
+      <c r="I1" s="59" t="e">
         <f>VLOOKUP('Tab 2'!A7, E1:F3, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L1" s="60">
+      <c r="L1" s="59">
         <v>1</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="60">
+      <c r="N1" s="59">
         <v>1</v>
       </c>
-      <c r="O1" s="60" t="e">
+      <c r="O1" s="59" t="e">
         <f t="shared" ref="O1:O12" si="0">IF(NOT($I$1 = $I$3), $M1, IF($J$2 &gt;= $N1, $M1, " "))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="59"/>
-      <c r="H2" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="I2" s="61"/>
-      <c r="J2" s="60" t="e">
+      <c r="B2" s="58"/>
+      <c r="H2" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="60"/>
+      <c r="J2" s="59" t="e">
         <f>VLOOKUP(I2, M1:N12, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L2" s="60">
+      <c r="L2" s="59">
         <v>2</v>
       </c>
-      <c r="M2" s="60" t="s">
+      <c r="M2" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="60">
+      <c r="N2" s="59">
         <v>2</v>
       </c>
-      <c r="O2" s="60" t="e">
+      <c r="O2" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="59"/>
-      <c r="H3" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="61"/>
-      <c r="L3" s="60">
+      <c r="B3" s="58"/>
+      <c r="H3" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="60"/>
+      <c r="L3" s="59">
         <v>3</v>
       </c>
-      <c r="M3" s="60" t="s">
+      <c r="M3" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="60">
+      <c r="N3" s="59">
         <v>3</v>
       </c>
-      <c r="O3" s="60" t="e">
+      <c r="O3" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="59"/>
-      <c r="H4" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I4" s="61"/>
-      <c r="L4" s="60">
+      <c r="B4" s="58"/>
+      <c r="H4" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="60"/>
+      <c r="L4" s="59">
         <v>4</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="60">
+      <c r="N4" s="59">
         <v>4</v>
       </c>
-      <c r="O4" s="60" t="e">
+      <c r="O4" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="59"/>
-      <c r="H5" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="60" t="e">
+      <c r="B5" s="58"/>
+      <c r="H5" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="60"/>
+      <c r="J5" s="59" t="e">
         <f>VLOOKUP($I$5, $B$1:$C$500, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" s="60">
+      <c r="L5" s="59">
         <v>5</v>
       </c>
-      <c r="M5" s="60" t="s">
+      <c r="M5" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="60">
+      <c r="N5" s="59">
         <v>5</v>
       </c>
-      <c r="O5" s="60" t="e">
+      <c r="O5" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="59"/>
-      <c r="L6" s="60">
+      <c r="B6" s="58"/>
+      <c r="L6" s="59">
         <v>6</v>
       </c>
-      <c r="M6" s="60" t="s">
+      <c r="M6" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="60">
+      <c r="N6" s="59">
         <v>6</v>
       </c>
-      <c r="O6" s="60" t="e">
+      <c r="O6" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="L7" s="60">
+      <c r="B7" s="58"/>
+      <c r="L7" s="59">
         <v>7</v>
       </c>
-      <c r="M7" s="60" t="s">
+      <c r="M7" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="60">
+      <c r="N7" s="59">
         <v>7</v>
       </c>
-      <c r="O7" s="60" t="e">
+      <c r="O7" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="59"/>
-      <c r="L8" s="60">
+      <c r="B8" s="58"/>
+      <c r="L8" s="59">
         <v>8</v>
       </c>
-      <c r="M8" s="60" t="s">
+      <c r="M8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="60">
+      <c r="N8" s="59">
         <v>8</v>
       </c>
-      <c r="O8" s="60" t="e">
+      <c r="O8" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="59"/>
-      <c r="L9" s="60">
+      <c r="B9" s="58"/>
+      <c r="L9" s="59">
         <v>9</v>
       </c>
-      <c r="M9" s="60" t="s">
+      <c r="M9" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="60">
+      <c r="N9" s="59">
         <v>9</v>
       </c>
-      <c r="O9" s="60" t="e">
+      <c r="O9" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="59"/>
-      <c r="L10" s="60">
+      <c r="B10" s="58"/>
+      <c r="L10" s="59">
         <v>10</v>
       </c>
-      <c r="M10" s="60" t="s">
+      <c r="M10" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="60">
+      <c r="N10" s="59">
         <v>10</v>
       </c>
-      <c r="O10" s="60" t="e">
+      <c r="O10" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="59"/>
-      <c r="L11" s="60">
+      <c r="B11" s="58"/>
+      <c r="L11" s="59">
         <v>11</v>
       </c>
-      <c r="M11" s="60" t="s">
+      <c r="M11" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="60">
+      <c r="N11" s="59">
         <v>11</v>
       </c>
-      <c r="O11" s="60" t="e">
+      <c r="O11" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="L12" s="60">
+      <c r="B12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="L12" s="59">
         <v>12</v>
       </c>
-      <c r="M12" s="60" t="s">
+      <c r="M12" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="60">
+      <c r="N12" s="59">
         <v>12</v>
       </c>
-      <c r="O12" s="60" t="e">
+      <c r="O12" s="59" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D13" s="62"/>
+      <c r="D13" s="61"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="59"/>
+      <c r="B25" s="58"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="59"/>
+      <c r="B26" s="58"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="59"/>
+      <c r="B27" s="58"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="59"/>
+      <c r="B28" s="58"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="59"/>
+      <c r="B29" s="58"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="59"/>
+      <c r="B30" s="58"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="59"/>
+      <c r="B31" s="58"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="59"/>
+      <c r="B32" s="58"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="59"/>
+      <c r="B33" s="58"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="59"/>
+      <c r="B34" s="58"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="59"/>
+      <c r="B35" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5683,19 +5678,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="57" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="57"/>
-    <col min="4" max="4" width="9.42578125" style="57" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="57"/>
-    <col min="6" max="6" width="18" style="57" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="57" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="57" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="1" width="14.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="56"/>
+    <col min="4" max="4" width="9.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="56"/>
+    <col min="6" max="6" width="18" style="56" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I1" s="58"/>
+      <c r="I1" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update link to glossary
</commit_message>
<xml_diff>
--- a/templates/discharges-template.xlsx
+++ b/templates/discharges-template.xlsx
@@ -673,15 +673,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -808,21 +805,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -843,6 +825,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3039,424 +3036,429 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="str">
+      <c r="A1" s="66" t="str">
         <f>"These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland."</f>
         <v>These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland.</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="10"/>
-      <c r="L1" s="18" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="9"/>
+      <c r="L1" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
       <c r="J8" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="50" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="49" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="22" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="68"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="68"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="68"/>
-      <c r="H11" s="68"/>
-      <c r="I11" s="68"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="62"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="62"/>
-      <c r="I14" s="62"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="5"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="11"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="11"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
     </row>
     <row r="21" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
     </row>
     <row r="22" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
     </row>
     <row r="23" spans="1:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
     </row>
     <row r="24" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
     </row>
     <row r="25" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A22:I22"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A12:H12"/>
@@ -3468,11 +3470,6 @@
     <mergeCell ref="A8:I8"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="A22:I22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A14" location="'Tab 1'!A1" display="Tab 1"/>
@@ -3502,7 +3499,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="40" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="39" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="7" width="12.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
@@ -3510,556 +3507,556 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="str">
+      <c r="B1" s="23" t="str">
         <f>Guide!A1</f>
         <v>These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland.</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="e">
+      <c r="B3" s="74" t="e">
         <f>"All delay reasons, "&amp; $A$6</f>
         <v>#NAME?</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-    </row>
-    <row r="4" spans="1:15" s="45" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46" t="str">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="1:15" s="44" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45" t="str">
         <f xml:space="preserve"> "Trend: " &amp; lookup!$I$2 &amp; " " &amp; (lookup!$I$4 - 2) &amp; " to " &amp; lookup!$I$2 &amp; " " &amp; lookup!$I$4</f>
         <v xml:space="preserve">Trend:  -2 to  </v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
+      <c r="L4" s="45"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
     </row>
     <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+      <c r="A5" s="37">
         <v>1</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
     </row>
     <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="e">
+      <c r="A6" s="39" t="e">
         <f>VLOOKUP($A$5, fy, 2, FALSE)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
+      <c r="C6" s="35"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="e">
+      <c r="A7" s="39" t="e">
         <f>LEFT($A$6, 4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="77"/>
-      <c r="E7" s="76" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="77"/>
-      <c r="G7" s="28"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="e">
+      <c r="A8" s="52" t="e">
         <f>"20"&amp;RIGHT($A$6, 2)</f>
         <v>#NAME?</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="G8" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="54" t="e">
+      <c r="A9" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B9, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B9" s="44" t="e">
+      <c r="B9" s="43" t="e">
         <f xml:space="preserve"> "April " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C9" s="51" t="str">
+      <c r="C9" s="50" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D9" s="29" t="str">
+      <c r="D9" s="28" t="str">
         <f t="shared" ref="D9:D20" si="0">IFERROR($C9/$G9, "-")</f>
         <v>-</v>
       </c>
-      <c r="E9" s="51" t="str">
+      <c r="E9" s="50" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F9" s="29" t="str">
+      <c r="F9" s="28" t="str">
         <f t="shared" ref="F9:F20" si="1">IFERROR($E9/$G9, "-")</f>
         <v>-</v>
       </c>
-      <c r="G9" s="51" t="str">
+      <c r="G9" s="50" t="str">
         <f>IFERROR(VLOOKUP($B9&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="e">
+      <c r="A10" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B10, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B10" s="44" t="e">
+      <c r="B10" s="43" t="e">
         <f xml:space="preserve"> "May " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C10" s="51" t="str">
+      <c r="C10" s="50" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D10" s="29" t="str">
+      <c r="D10" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E10" s="51" t="str">
+      <c r="E10" s="50" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F10" s="29" t="str">
+      <c r="F10" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G10" s="51" t="str">
+      <c r="G10" s="50" t="str">
         <f>IFERROR(VLOOKUP($B10&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="e">
+      <c r="A11" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B11, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B11" s="44" t="e">
+      <c r="B11" s="43" t="e">
         <f xml:space="preserve"> "June " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C11" s="51" t="str">
+      <c r="C11" s="50" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D11" s="29" t="str">
+      <c r="D11" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E11" s="51" t="str">
+      <c r="E11" s="50" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F11" s="29" t="str">
+      <c r="F11" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G11" s="51" t="str">
+      <c r="G11" s="50" t="str">
         <f>IFERROR(VLOOKUP($B11&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="54" t="e">
+      <c r="A12" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B12, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B12" s="44" t="e">
+      <c r="B12" s="43" t="e">
         <f xml:space="preserve"> "July " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C12" s="51" t="str">
+      <c r="C12" s="50" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D12" s="29" t="str">
+      <c r="D12" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E12" s="51" t="str">
+      <c r="E12" s="50" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F12" s="29" t="str">
+      <c r="F12" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G12" s="51" t="str">
+      <c r="G12" s="50" t="str">
         <f>IFERROR(VLOOKUP($B12&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="e">
+      <c r="A13" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B13, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B13" s="44" t="e">
+      <c r="B13" s="43" t="e">
         <f xml:space="preserve"> "August " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C13" s="51" t="str">
+      <c r="C13" s="50" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D13" s="29" t="str">
+      <c r="D13" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E13" s="51" t="str">
+      <c r="E13" s="50" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F13" s="29" t="str">
+      <c r="F13" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G13" s="51" t="str">
+      <c r="G13" s="50" t="str">
         <f>IFERROR(VLOOKUP($B13&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="54" t="e">
+      <c r="A14" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B14, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B14" s="44" t="e">
+      <c r="B14" s="43" t="e">
         <f xml:space="preserve"> "September " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C14" s="51" t="str">
+      <c r="C14" s="50" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D14" s="29" t="str">
+      <c r="D14" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E14" s="51" t="str">
+      <c r="E14" s="50" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F14" s="29" t="str">
+      <c r="F14" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G14" s="51" t="str">
+      <c r="G14" s="50" t="str">
         <f>IFERROR(VLOOKUP($B14&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="e">
+      <c r="A15" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B15, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B15" s="44" t="e">
+      <c r="B15" s="43" t="e">
         <f xml:space="preserve"> "October " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C15" s="51" t="str">
+      <c r="C15" s="50" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D15" s="29" t="str">
+      <c r="D15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E15" s="51" t="str">
+      <c r="E15" s="50" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F15" s="29" t="str">
+      <c r="F15" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G15" s="51" t="str">
+      <c r="G15" s="50" t="str">
         <f>IFERROR(VLOOKUP($B15&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="e">
+      <c r="A16" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B16, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B16" s="44" t="e">
+      <c r="B16" s="43" t="e">
         <f xml:space="preserve"> "November " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C16" s="51" t="str">
+      <c r="C16" s="50" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D16" s="29" t="str">
+      <c r="D16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E16" s="51" t="str">
+      <c r="E16" s="50" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F16" s="29" t="str">
+      <c r="F16" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G16" s="51" t="str">
+      <c r="G16" s="50" t="str">
         <f>IFERROR(VLOOKUP($B16&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="54" t="e">
+      <c r="A17" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B17, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B17" s="44" t="e">
+      <c r="B17" s="43" t="e">
         <f xml:space="preserve"> "December " &amp; $A$7</f>
         <v>#NAME?</v>
       </c>
-      <c r="C17" s="51" t="str">
+      <c r="C17" s="50" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D17" s="29" t="str">
+      <c r="D17" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E17" s="51" t="str">
+      <c r="E17" s="50" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F17" s="29" t="str">
+      <c r="F17" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G17" s="51" t="str">
+      <c r="G17" s="50" t="str">
         <f>IFERROR(VLOOKUP($B17&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="e">
+      <c r="A18" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B18, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B18" s="44" t="e">
+      <c r="B18" s="43" t="e">
         <f xml:space="preserve"> "January " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C18" s="51" t="str">
+      <c r="C18" s="50" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D18" s="29" t="str">
+      <c r="D18" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E18" s="51" t="str">
+      <c r="E18" s="50" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F18" s="29" t="str">
+      <c r="F18" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G18" s="51" t="str">
+      <c r="G18" s="50" t="str">
         <f>IFERROR(VLOOKUP($B18&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="e">
+      <c r="A19" s="53" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B19, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B19" s="44" t="e">
+      <c r="B19" s="43" t="e">
         <f xml:space="preserve"> "February " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C19" s="51" t="str">
+      <c r="C19" s="50" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D19" s="29" t="str">
+      <c r="D19" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E19" s="51" t="str">
+      <c r="E19" s="50" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F19" s="29" t="str">
+      <c r="F19" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G19" s="51" t="str">
+      <c r="G19" s="50" t="str">
         <f>IFERROR(VLOOKUP($B19&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="e">
+      <c r="A20" s="54" t="e">
         <f>_xlfn.IFNA(VLOOKUP($B20, months, 2, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="B20" s="44" t="e">
+      <c r="B20" s="43" t="e">
         <f xml:space="preserve"> "March " &amp; $A$8</f>
         <v>#NAME?</v>
       </c>
-      <c r="C20" s="51" t="str">
+      <c r="C20" s="50" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 4, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="D20" s="29" t="str">
+      <c r="D20" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E20" s="51" t="str">
+      <c r="E20" s="50" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 5, FALSE), "-")</f>
         <v>-</v>
       </c>
-      <c r="F20" s="29" t="str">
+      <c r="F20" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G20" s="51" t="str">
+      <c r="G20" s="50" t="str">
         <f>IFERROR(VLOOKUP($B20&amp;"Scotland", data, 6, FALSE), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="47" t="str">
+      <c r="B22" s="46" t="str">
         <f>"Information is currently available up to " &amp; lookup!$I$5</f>
         <v xml:space="preserve">Information is currently available up to </v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="32" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="31" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
     </row>
     <row r="31" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4121,543 +4118,543 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="40" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="39" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="24" t="str">
+      <c r="B1" s="23" t="str">
         <f>Guide!A1</f>
         <v>These data are for management purposes only. Please treat the material and any indication of the results as restricted until public release by Public Health Scotland.</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="e">
+      <c r="B2" s="74" t="e">
         <f>"Tab 2 - Discharges from hospital following period of delay to Home or to Placement; by Health Board; " &amp; A12</f>
         <v>#NAME?</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.25">
-      <c r="B4" s="41"/>
+      <c r="B4" s="40"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="35" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="37">
+      <c r="A7" s="36">
         <v>1</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="e">
+      <c r="A8" s="37" t="e">
         <f>VLOOKUP($A$7, fy, 2, FALSE)</f>
         <v>#NAME?</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="76" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="77"/>
-      <c r="E8" s="76" t="s">
+      <c r="D8" s="76"/>
+      <c r="E8" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="77"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:15" ht="27" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+      <c r="A9" s="36">
         <v>11</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="25" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="str">
+      <c r="A10" s="36" t="str">
         <f>VLOOKUP(A9, lookup!L1:M12, 2, FALSE)</f>
         <v>February</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="49" t="e">
+      <c r="C10" s="48" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B10, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D10" s="35" t="str">
+      <c r="D10" s="34" t="str">
         <f>IFERROR(C10/G10, "-")</f>
         <v>-</v>
       </c>
-      <c r="E10" s="49" t="e">
+      <c r="E10" s="48" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B10, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F10" s="35" t="str">
+      <c r="F10" s="34" t="str">
         <f>IFERROR(E10/G10, "-")</f>
         <v>-</v>
       </c>
-      <c r="G10" s="49" t="e">
+      <c r="G10" s="48" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B10, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="36"/>
+      <c r="B11" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="51" t="e">
+      <c r="C11" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D11" s="29" t="str">
+      <c r="D11" s="28" t="str">
         <f>IFERROR(C11/G11, "-")</f>
         <v>-</v>
       </c>
-      <c r="E11" s="51" t="e">
+      <c r="E11" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F11" s="29" t="str">
+      <c r="F11" s="28" t="str">
         <f>IFERROR(E11/G11, "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="51" t="e">
+      <c r="G11" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B11, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="e">
+      <c r="A12" s="36" t="e">
         <f>IF(A9&lt;10, A10 &amp; " " &amp; LEFT(A8, 4), A10 &amp; " 20" &amp; RIGHT(A8, 2))</f>
         <v>#NAME?</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="51" t="e">
+      <c r="C12" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D12" s="29" t="str">
+      <c r="D12" s="28" t="str">
         <f t="shared" ref="D12:D24" si="0">IFERROR(C12/G12, "-")</f>
         <v>-</v>
       </c>
-      <c r="E12" s="51" t="e">
+      <c r="E12" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F12" s="29" t="str">
+      <c r="F12" s="28" t="str">
         <f t="shared" ref="F12:F24" si="1">IFERROR(E12/G12, "-")</f>
         <v>-</v>
       </c>
-      <c r="G12" s="51" t="e">
+      <c r="G12" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B12, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="51" t="e">
+      <c r="C13" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D13" s="29" t="str">
+      <c r="D13" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E13" s="51" t="e">
+      <c r="E13" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F13" s="29" t="str">
+      <c r="F13" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G13" s="51" t="e">
+      <c r="G13" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B13, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="51" t="e">
+      <c r="C14" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D14" s="29" t="str">
+      <c r="D14" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E14" s="51" t="e">
+      <c r="E14" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F14" s="29" t="str">
+      <c r="F14" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G14" s="51" t="e">
+      <c r="G14" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B14, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="51" t="e">
+      <c r="C15" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D15" s="29" t="str">
+      <c r="D15" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E15" s="51" t="e">
+      <c r="E15" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F15" s="29" t="str">
+      <c r="F15" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G15" s="51" t="e">
+      <c r="G15" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B15, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="51" t="e">
+      <c r="C16" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D16" s="29" t="str">
+      <c r="D16" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E16" s="51" t="e">
+      <c r="E16" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F16" s="29" t="str">
+      <c r="F16" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G16" s="51" t="e">
+      <c r="G16" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B16, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="51" t="e">
+      <c r="C17" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D17" s="29" t="str">
+      <c r="D17" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E17" s="51" t="e">
+      <c r="E17" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F17" s="29" t="str">
+      <c r="F17" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G17" s="51" t="e">
+      <c r="G17" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B17, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="51" t="e">
+      <c r="C18" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D18" s="29" t="str">
+      <c r="D18" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E18" s="51" t="e">
+      <c r="E18" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F18" s="29" t="str">
+      <c r="F18" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G18" s="51" t="e">
+      <c r="G18" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B18, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="51" t="e">
+      <c r="C19" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D19" s="29" t="str">
+      <c r="D19" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E19" s="51" t="e">
+      <c r="E19" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F19" s="29" t="str">
+      <c r="F19" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G19" s="51" t="e">
+      <c r="G19" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B19, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="51" t="e">
+      <c r="C20" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D20" s="29" t="str">
+      <c r="D20" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E20" s="51" t="e">
+      <c r="E20" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F20" s="29" t="str">
+      <c r="F20" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G20" s="51" t="e">
+      <c r="G20" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B20, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="51" t="e">
+      <c r="C21" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D21" s="29" t="str">
+      <c r="D21" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E21" s="51" t="e">
+      <c r="E21" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F21" s="29" t="str">
+      <c r="F21" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G21" s="51" t="e">
+      <c r="G21" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B21, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="51" t="e">
+      <c r="C22" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D22" s="29" t="str">
+      <c r="D22" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E22" s="51" t="e">
+      <c r="E22" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F22" s="29" t="str">
+      <c r="F22" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G22" s="51" t="e">
+      <c r="G22" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B22, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="51" t="e">
+      <c r="C23" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D23" s="29" t="str">
+      <c r="D23" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E23" s="51" t="e">
+      <c r="E23" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F23" s="29" t="str">
+      <c r="F23" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G23" s="51" t="e">
+      <c r="G23" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B23, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="51" t="e">
+      <c r="C24" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 4, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="D24" s="29" t="str">
+      <c r="D24" s="28" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
-      <c r="E24" s="51" t="e">
+      <c r="E24" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 5, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
-      <c r="F24" s="29" t="str">
+      <c r="F24" s="28" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="G24" s="51" t="e">
+      <c r="G24" s="50" t="e">
         <f>_xlfn.IFNA(VLOOKUP($A$12&amp;$B24, data, 6, FALSE), "-")</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="48" t="str">
+      <c r="B26" s="47" t="str">
         <f>"Information is currently available up to "&amp;LEFT(lookup!I2,3)&amp;"-"&amp;lookup!I4</f>
         <v>Information is currently available up to -</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="str">
+      <c r="B28" s="32" t="str">
         <f>'Tab 1'!B24</f>
         <v>Notes</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="32" t="str">
+      <c r="B29" s="31" t="str">
         <f>'Tab 1'!B25</f>
         <v>1. Home includes discharges home, and discharges home with support.</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="str">
+      <c r="B30" s="31" t="str">
         <f>'Tab 1'!B26</f>
         <v>2. Placement includes discharges to care home, and other placements including Intermediate Care.</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="78" t="str">
+      <c r="B31" s="77" t="str">
         <f>'Tab 1'!B27</f>
         <v>3. These figures are a subset of the total number of discharges from hospital and include only those people who experienced a period of delay prior to their discharge and were discharged home or to a placement (delays in hospital that ended due to death are not included).</v>
       </c>
-      <c r="C31" s="78"/>
-      <c r="D31" s="78"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4731,286 +4728,286 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="3" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="59" customWidth="1"/>
-    <col min="5" max="5" width="2" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="59" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="59" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="59"/>
-    <col min="12" max="12" width="3" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="59" customWidth="1"/>
-    <col min="14" max="14" width="3" style="59" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.85546875" style="59" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="59"/>
-    <col min="18" max="18" width="15.42578125" style="59" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="3" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="3" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="58" customWidth="1"/>
+    <col min="5" max="5" width="2" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="58" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="58" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="58"/>
+    <col min="12" max="12" width="3" style="58" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="58" customWidth="1"/>
+    <col min="14" max="14" width="3" style="58" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="58" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="58"/>
+    <col min="18" max="18" width="15.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="58"/>
-      <c r="H1" s="59" t="s">
+      <c r="B1" s="57"/>
+      <c r="H1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="59" t="e">
+      <c r="I1" s="58" t="e">
         <f>VLOOKUP('Tab 2'!A7, E1:F3, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L1" s="59">
+      <c r="L1" s="58">
         <v>1</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="59">
+      <c r="N1" s="58">
         <v>1</v>
       </c>
-      <c r="O1" s="59" t="e">
+      <c r="O1" s="58" t="e">
         <f t="shared" ref="O1:O12" si="0">IF(NOT($I$1 = $I$3), $M1, IF($J$2 &gt;= $N1, $M1, " "))</f>
         <v>#N/A</v>
       </c>
     </row>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="58"/>
-      <c r="H2" s="59" t="s">
+      <c r="B2" s="57"/>
+      <c r="H2" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="59" t="e">
+      <c r="I2" s="59"/>
+      <c r="J2" s="58" t="e">
         <f>VLOOKUP(I2, M1:N12, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L2" s="59">
+      <c r="L2" s="58">
         <v>2</v>
       </c>
-      <c r="M2" s="59" t="s">
+      <c r="M2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="59">
+      <c r="N2" s="58">
         <v>2</v>
       </c>
-      <c r="O2" s="59" t="e">
+      <c r="O2" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="58"/>
-      <c r="H3" s="59" t="s">
+      <c r="B3" s="57"/>
+      <c r="H3" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="L3" s="59">
+      <c r="I3" s="59"/>
+      <c r="L3" s="58">
         <v>3</v>
       </c>
-      <c r="M3" s="59" t="s">
+      <c r="M3" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="59">
+      <c r="N3" s="58">
         <v>3</v>
       </c>
-      <c r="O3" s="59" t="e">
+      <c r="O3" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
-      <c r="H4" s="59" t="s">
+      <c r="B4" s="57"/>
+      <c r="H4" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="L4" s="59">
+      <c r="I4" s="59"/>
+      <c r="L4" s="58">
         <v>4</v>
       </c>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="N4" s="59">
+      <c r="N4" s="58">
         <v>4</v>
       </c>
-      <c r="O4" s="59" t="e">
+      <c r="O4" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="58"/>
-      <c r="H5" s="59" t="s">
+      <c r="B5" s="57"/>
+      <c r="H5" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="59" t="e">
+      <c r="I5" s="59"/>
+      <c r="J5" s="58" t="e">
         <f>VLOOKUP($I$5, $B$1:$C$500, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L5" s="59">
+      <c r="L5" s="58">
         <v>5</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="M5" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="59">
+      <c r="N5" s="58">
         <v>5</v>
       </c>
-      <c r="O5" s="59" t="e">
+      <c r="O5" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
-      <c r="L6" s="59">
+      <c r="B6" s="57"/>
+      <c r="L6" s="58">
         <v>6</v>
       </c>
-      <c r="M6" s="59" t="s">
+      <c r="M6" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="59">
+      <c r="N6" s="58">
         <v>6</v>
       </c>
-      <c r="O6" s="59" t="e">
+      <c r="O6" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="58"/>
-      <c r="L7" s="59">
+      <c r="B7" s="57"/>
+      <c r="L7" s="58">
         <v>7</v>
       </c>
-      <c r="M7" s="59" t="s">
+      <c r="M7" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="59">
+      <c r="N7" s="58">
         <v>7</v>
       </c>
-      <c r="O7" s="59" t="e">
+      <c r="O7" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="L8" s="59">
+      <c r="B8" s="57"/>
+      <c r="L8" s="58">
         <v>8</v>
       </c>
-      <c r="M8" s="59" t="s">
+      <c r="M8" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="59">
+      <c r="N8" s="58">
         <v>8</v>
       </c>
-      <c r="O8" s="59" t="e">
+      <c r="O8" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="L9" s="59">
+      <c r="B9" s="57"/>
+      <c r="L9" s="58">
         <v>9</v>
       </c>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="59">
+      <c r="N9" s="58">
         <v>9</v>
       </c>
-      <c r="O9" s="59" t="e">
+      <c r="O9" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="58"/>
-      <c r="L10" s="59">
+      <c r="B10" s="57"/>
+      <c r="L10" s="58">
         <v>10</v>
       </c>
-      <c r="M10" s="59" t="s">
+      <c r="M10" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="59">
+      <c r="N10" s="58">
         <v>10</v>
       </c>
-      <c r="O10" s="59" t="e">
+      <c r="O10" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
-      <c r="L11" s="59">
+      <c r="B11" s="57"/>
+      <c r="L11" s="58">
         <v>11</v>
       </c>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="N11" s="59">
+      <c r="N11" s="58">
         <v>11</v>
       </c>
-      <c r="O11" s="59" t="e">
+      <c r="O11" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="L12" s="59">
+      <c r="B12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="L12" s="58">
         <v>12</v>
       </c>
-      <c r="M12" s="59" t="s">
+      <c r="M12" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="59">
+      <c r="N12" s="58">
         <v>12</v>
       </c>
-      <c r="O12" s="59" t="e">
+      <c r="O12" s="58" t="e">
         <f t="shared" si="0"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D13" s="61"/>
+      <c r="D13" s="60"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="58"/>
+      <c r="B25" s="57"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="58"/>
+      <c r="B26" s="57"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="58"/>
+      <c r="B27" s="57"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="58"/>
+      <c r="B28" s="57"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="58"/>
+      <c r="B29" s="57"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="58"/>
+      <c r="B30" s="57"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="58"/>
+      <c r="B31" s="57"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="58"/>
+      <c r="B32" s="57"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="58"/>
+      <c r="B33" s="57"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="58"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="58"/>
+      <c r="B35" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5035,634 +5032,634 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="39"/>
+      <c r="B2" s="38"/>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="39"/>
+      <c r="B3" s="38"/>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="39"/>
+      <c r="B4" s="38"/>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="39"/>
+      <c r="B5" s="38"/>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="39"/>
+      <c r="B6" s="38"/>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="39"/>
+      <c r="B7" s="38"/>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
+      <c r="B8" s="38"/>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="39"/>
+      <c r="B9" s="38"/>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="39"/>
+      <c r="B10" s="38"/>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="39"/>
+      <c r="B11" s="38"/>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
+      <c r="B12" s="38"/>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
+      <c r="B13" s="38"/>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="39"/>
+      <c r="B14" s="38"/>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
+      <c r="B15" s="38"/>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="38"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+      <c r="B17" s="38"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="38"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="39"/>
+      <c r="B19" s="38"/>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+      <c r="B20" s="38"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="38"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
+      <c r="B22" s="38"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="39"/>
+      <c r="B23" s="38"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="39"/>
+      <c r="B24" s="38"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="39"/>
+      <c r="B25" s="38"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="39"/>
+      <c r="B26" s="38"/>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="39"/>
+      <c r="B27" s="38"/>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="39"/>
+      <c r="B28" s="38"/>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="39"/>
+      <c r="B29" s="38"/>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="39"/>
+      <c r="B30" s="38"/>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="39"/>
+      <c r="B31" s="38"/>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="39"/>
+      <c r="B32" s="38"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="39"/>
+      <c r="B33" s="38"/>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="39"/>
+      <c r="B34" s="38"/>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="39"/>
+      <c r="B35" s="38"/>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="39"/>
+      <c r="B36" s="38"/>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="39"/>
+      <c r="B37" s="38"/>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="39"/>
+      <c r="B38" s="38"/>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="39"/>
+      <c r="B39" s="38"/>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="39"/>
+      <c r="B40" s="38"/>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="39"/>
+      <c r="B41" s="38"/>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="39"/>
+      <c r="B42" s="38"/>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="39"/>
+      <c r="B43" s="38"/>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="39"/>
+      <c r="B44" s="38"/>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="39"/>
+      <c r="B45" s="38"/>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="39"/>
+      <c r="B46" s="38"/>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="39"/>
+      <c r="B47" s="38"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="39"/>
+      <c r="B48" s="38"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="39"/>
+      <c r="B49" s="38"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="39"/>
+      <c r="B50" s="38"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="39"/>
+      <c r="B51" s="38"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="39"/>
+      <c r="B52" s="38"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="39"/>
+      <c r="B53" s="38"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="39"/>
+      <c r="B54" s="38"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="39"/>
+      <c r="B55" s="38"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="39"/>
+      <c r="B56" s="38"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="39"/>
+      <c r="B57" s="38"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="39"/>
+      <c r="B58" s="38"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="39"/>
+      <c r="B59" s="38"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="39"/>
+      <c r="B60" s="38"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="39"/>
+      <c r="B61" s="38"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="39"/>
+      <c r="B62" s="38"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="39"/>
+      <c r="B63" s="38"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="39"/>
+      <c r="B64" s="38"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="39"/>
+      <c r="B65" s="38"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="39"/>
+      <c r="B66" s="38"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="39"/>
+      <c r="B67" s="38"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="39"/>
+      <c r="B68" s="38"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="39"/>
+      <c r="B69" s="38"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="39"/>
+      <c r="B70" s="38"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="39"/>
+      <c r="B71" s="38"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="39"/>
+      <c r="B72" s="38"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="39"/>
+      <c r="B73" s="38"/>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="39"/>
+      <c r="B74" s="38"/>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="39"/>
+      <c r="B75" s="38"/>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="39"/>
+      <c r="B76" s="38"/>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="39"/>
+      <c r="B77" s="38"/>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="39"/>
+      <c r="B78" s="38"/>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="39"/>
+      <c r="B79" s="38"/>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="39"/>
+      <c r="B80" s="38"/>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="39"/>
+      <c r="B81" s="38"/>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="39"/>
+      <c r="B82" s="38"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="39"/>
+      <c r="B83" s="38"/>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="39"/>
+      <c r="B84" s="38"/>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="39"/>
+      <c r="B85" s="38"/>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="39"/>
+      <c r="B86" s="38"/>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="39"/>
+      <c r="B87" s="38"/>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="39"/>
+      <c r="B88" s="38"/>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="39"/>
+      <c r="B89" s="38"/>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="39"/>
+      <c r="B90" s="38"/>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="39"/>
+      <c r="B91" s="38"/>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="39"/>
+      <c r="B92" s="38"/>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="39"/>
+      <c r="B93" s="38"/>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="39"/>
+      <c r="B94" s="38"/>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="39"/>
+      <c r="B95" s="38"/>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="39"/>
+      <c r="B96" s="38"/>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="39"/>
+      <c r="B97" s="38"/>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="39"/>
+      <c r="B98" s="38"/>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="39"/>
+      <c r="B99" s="38"/>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="39"/>
+      <c r="B100" s="38"/>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="39"/>
+      <c r="B101" s="38"/>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="39"/>
+      <c r="B102" s="38"/>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="39"/>
+      <c r="B103" s="38"/>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="39"/>
+      <c r="B104" s="38"/>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="39"/>
+      <c r="B105" s="38"/>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="39"/>
+      <c r="B106" s="38"/>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="39"/>
+      <c r="B107" s="38"/>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="39"/>
+      <c r="B108" s="38"/>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="39"/>
+      <c r="B109" s="38"/>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="39"/>
+      <c r="B110" s="38"/>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="39"/>
+      <c r="B111" s="38"/>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="39"/>
+      <c r="B112" s="38"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="39"/>
+      <c r="B113" s="38"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="39"/>
+      <c r="B114" s="38"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="39"/>
+      <c r="B115" s="38"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="39"/>
+      <c r="B116" s="38"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="39"/>
+      <c r="B117" s="38"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="39"/>
+      <c r="B118" s="38"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="39"/>
+      <c r="B119" s="38"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="39"/>
+      <c r="B120" s="38"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="39"/>
+      <c r="B121" s="38"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="39"/>
+      <c r="B122" s="38"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="39"/>
+      <c r="B123" s="38"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="39"/>
+      <c r="B124" s="38"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="39"/>
+      <c r="B125" s="38"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="39"/>
+      <c r="B126" s="38"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="39"/>
+      <c r="B127" s="38"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="39"/>
+      <c r="B128" s="38"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="39"/>
+      <c r="B129" s="38"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="39"/>
+      <c r="B130" s="38"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="39"/>
+      <c r="B131" s="38"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="39"/>
+      <c r="B132" s="38"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="39"/>
+      <c r="B133" s="38"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="39"/>
+      <c r="B134" s="38"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="39"/>
+      <c r="B135" s="38"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="39"/>
+      <c r="B136" s="38"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="39"/>
+      <c r="B137" s="38"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="39"/>
+      <c r="B138" s="38"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="39"/>
+      <c r="B139" s="38"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="39"/>
+      <c r="B140" s="38"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="39"/>
+      <c r="B141" s="38"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="39"/>
+      <c r="B142" s="38"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="39"/>
+      <c r="B143" s="38"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="39"/>
+      <c r="B144" s="38"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="39"/>
+      <c r="B145" s="38"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="39"/>
+      <c r="B146" s="38"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="39"/>
+      <c r="B147" s="38"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="39"/>
+      <c r="B148" s="38"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="39"/>
+      <c r="B149" s="38"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="39"/>
+      <c r="B150" s="38"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="39"/>
+      <c r="B151" s="38"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="39"/>
+      <c r="B152" s="38"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="39"/>
+      <c r="B153" s="38"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="39"/>
+      <c r="B154" s="38"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="39"/>
+      <c r="B155" s="38"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="39"/>
+      <c r="B156" s="38"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="39"/>
+      <c r="B157" s="38"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="39"/>
+      <c r="B158" s="38"/>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="39"/>
+      <c r="B159" s="38"/>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="39"/>
+      <c r="B160" s="38"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="39"/>
+      <c r="B161" s="38"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="39"/>
+      <c r="B162" s="38"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="39"/>
+      <c r="B163" s="38"/>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="39"/>
+      <c r="B164" s="38"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="39"/>
+      <c r="B165" s="38"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="39"/>
+      <c r="B166" s="38"/>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="39"/>
+      <c r="B167" s="38"/>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="39"/>
+      <c r="B168" s="38"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="39"/>
+      <c r="B169" s="38"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="39"/>
+      <c r="B170" s="38"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="39"/>
+      <c r="B171" s="38"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="39"/>
+      <c r="B172" s="38"/>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="39"/>
+      <c r="B173" s="38"/>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="39"/>
+      <c r="B174" s="38"/>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="39"/>
+      <c r="B175" s="38"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="39"/>
+      <c r="B176" s="38"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="39"/>
+      <c r="B177" s="38"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="39"/>
+      <c r="B178" s="38"/>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="39"/>
+      <c r="B179" s="38"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="39"/>
+      <c r="B180" s="38"/>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="39"/>
+      <c r="B181" s="38"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="39"/>
+      <c r="B182" s="38"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="39"/>
+      <c r="B183" s="38"/>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="39"/>
+      <c r="B184" s="38"/>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="39"/>
+      <c r="B185" s="38"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="39"/>
+      <c r="B186" s="38"/>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B187" s="39"/>
+      <c r="B187" s="38"/>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B188" s="39"/>
+      <c r="B188" s="38"/>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B189" s="39"/>
+      <c r="B189" s="38"/>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B190" s="39"/>
+      <c r="B190" s="38"/>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B191" s="39"/>
+      <c r="B191" s="38"/>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B192" s="39"/>
+      <c r="B192" s="38"/>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B193" s="39"/>
+      <c r="B193" s="38"/>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B194" s="39"/>
+      <c r="B194" s="38"/>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B195" s="39"/>
+      <c r="B195" s="38"/>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B196" s="39"/>
+      <c r="B196" s="38"/>
     </row>
     <row r="437" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B437" s="43"/>
+      <c r="B437" s="42"/>
     </row>
     <row r="438" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B438" s="43"/>
+      <c r="B438" s="42"/>
     </row>
     <row r="439" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B439" s="43"/>
+      <c r="B439" s="42"/>
     </row>
     <row r="440" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B440" s="43"/>
+      <c r="B440" s="42"/>
     </row>
     <row r="441" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B441" s="43"/>
+      <c r="B441" s="42"/>
     </row>
     <row r="442" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B442" s="43"/>
+      <c r="B442" s="42"/>
     </row>
     <row r="443" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B443" s="43"/>
+      <c r="B443" s="42"/>
     </row>
     <row r="444" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B444" s="43"/>
+      <c r="B444" s="42"/>
     </row>
     <row r="445" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B445" s="43"/>
+      <c r="B445" s="42"/>
     </row>
     <row r="446" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B446" s="43"/>
+      <c r="B446" s="42"/>
     </row>
     <row r="447" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B447" s="43"/>
+      <c r="B447" s="42"/>
     </row>
     <row r="448" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B448" s="43"/>
+      <c r="B448" s="42"/>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B449" s="43"/>
+      <c r="B449" s="42"/>
     </row>
     <row r="450" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B450" s="43"/>
+      <c r="B450" s="42"/>
     </row>
     <row r="451" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B451" s="43"/>
+      <c r="B451" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5678,19 +5675,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="56" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="56" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="56"/>
-    <col min="4" max="4" width="9.42578125" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="56"/>
-    <col min="6" max="6" width="18" style="56" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="56" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="56" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="56"/>
+    <col min="1" max="1" width="14.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="55"/>
+    <col min="4" max="4" width="9.42578125" style="55" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="55"/>
+    <col min="6" max="6" width="18" style="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="55" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="55"/>
   </cols>
   <sheetData>
     <row r="1" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I1" s="57"/>
+      <c r="I1" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>